<commit_message>
Seasonal Awards, CN/JavaTPoint/1, DS/JavaTPoint/1, DE/JavaTPoint/1
</commit_message>
<xml_diff>
--- a/Z) EASTER EGGS/Seasonal Awards/Summary List.xlsx
+++ b/Z) EASTER EGGS/Seasonal Awards/Summary List.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0_MyFiles\BRIDGE BETWEEN BOTH\NOTEWORKS\AGENT OF FREEDOM\Seasonal Awards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91966\OneDrive\Desktop\Instant Codes\Cloned Repositaries\Noteworks\Z) EASTER EGGS\Seasonal Awards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED9A86C-1BB9-4046-9A0A-D1280E69C939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4666C78-0CAC-41AE-91D1-B3AC6B000F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
   <si>
     <t>SNO</t>
   </si>
@@ -153,9 +162,6 @@
     <t>Kaushal Patel</t>
   </si>
   <si>
-    <t>Counter-Strike 2</t>
-  </si>
-  <si>
     <t>The Butterfly Effect</t>
   </si>
   <si>
@@ -183,9 +189,6 @@
     <t>Ansh Tank Vipin</t>
   </si>
   <si>
-    <t>Robert Oppenheimer</t>
-  </si>
-  <si>
     <t>Jasmine Mansuri</t>
   </si>
   <si>
@@ -262,13 +265,88 @@
   </si>
   <si>
     <t>ChatGPT</t>
+  </si>
+  <si>
+    <t>Asphalt 9: Legends</t>
+  </si>
+  <si>
+    <t>Fall Guys</t>
+  </si>
+  <si>
+    <t>Theory Of Computation</t>
+  </si>
+  <si>
+    <t>Jurassic Park Ambience</t>
+  </si>
+  <si>
+    <t>Tosbit</t>
+  </si>
+  <si>
+    <t>Robert J. Oppenheimer</t>
+  </si>
+  <si>
+    <t>Amar Chandra</t>
+  </si>
+  <si>
+    <t>JavaTPoint</t>
+  </si>
+  <si>
+    <t>Mark Watney</t>
+  </si>
+  <si>
+    <t>Bear Grylls</t>
+  </si>
+  <si>
+    <t>Saving Private Ryan</t>
+  </si>
+  <si>
+    <t>OFF TOPIC</t>
+  </si>
+  <si>
+    <t>Paleontology</t>
+  </si>
+  <si>
+    <t>Western Philosophy</t>
+  </si>
+  <si>
+    <t>Jungian Topology</t>
+  </si>
+  <si>
+    <t>Eastern Philosophy</t>
+  </si>
+  <si>
+    <t>Science Fiction Movies</t>
+  </si>
+  <si>
+    <t>Quebec</t>
+  </si>
+  <si>
+    <t>SLOGAN</t>
+  </si>
+  <si>
+    <t>"Question the convention"</t>
+  </si>
+  <si>
+    <t>"Embrace your intelligence"</t>
+  </si>
+  <si>
+    <t>"Stand out with your talent"</t>
+  </si>
+  <si>
+    <t>"Compete and conquer"</t>
+  </si>
+  <si>
+    <t>"Forgive yourself"</t>
+  </si>
+  <si>
+    <t>"Broaden your mind"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,8 +362,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +424,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,6 +561,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -750,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,14 +880,16 @@
     <col min="9" max="9" width="20.453125" customWidth="1"/>
     <col min="10" max="10" width="30.26953125" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="20.26953125" customWidth="1"/>
+    <col min="12" max="12" width="22.453125" customWidth="1"/>
     <col min="13" max="13" width="21.90625" customWidth="1"/>
     <col min="14" max="14" width="17.36328125" customWidth="1"/>
     <col min="15" max="15" width="11.6328125" customWidth="1"/>
     <col min="16" max="16" width="21.08984375" customWidth="1"/>
+    <col min="17" max="17" width="23.6328125" customWidth="1"/>
+    <col min="18" max="18" width="29.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -820,13 +933,19 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -864,19 +983,25 @@
         <v>26</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -914,19 +1039,25 @@
         <v>31</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>32</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="R3" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -961,22 +1092,28 @@
         <v>39</v>
       </c>
       <c r="L4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>41</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="R4" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -987,46 +1124,52 @@
         <v>13</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="G5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="K5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="O5" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="R5" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1037,64 +1180,108 @@
         <v>19</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="20" t="s">
+      <c r="H6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="J6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="K6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="L6" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>62</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P6" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="R6" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2024</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="14"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E7" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="R7" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="8"/>
       <c r="C8" s="11"/>
@@ -1111,8 +1298,10 @@
       <c r="N8" s="8"/>
       <c r="O8" s="11"/>
       <c r="P8" s="14"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q8" s="23"/>
+      <c r="R8" s="25"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="8"/>
       <c r="C9" s="11"/>
@@ -1129,8 +1318,10 @@
       <c r="N9" s="8"/>
       <c r="O9" s="11"/>
       <c r="P9" s="14"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q9" s="23"/>
+      <c r="R9" s="25"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="8"/>
       <c r="C10" s="11"/>
@@ -1147,8 +1338,10 @@
       <c r="N10" s="8"/>
       <c r="O10" s="11"/>
       <c r="P10" s="14"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q10" s="23"/>
+      <c r="R10" s="25"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="8"/>
       <c r="C11" s="11"/>
@@ -1165,8 +1358,10 @@
       <c r="N11" s="8"/>
       <c r="O11" s="11"/>
       <c r="P11" s="14"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q11" s="23"/>
+      <c r="R11" s="25"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="8"/>
       <c r="C12" s="11"/>
@@ -1183,8 +1378,10 @@
       <c r="N12" s="8"/>
       <c r="O12" s="11"/>
       <c r="P12" s="14"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q12" s="23"/>
+      <c r="R12" s="25"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="8"/>
       <c r="C13" s="11"/>
@@ -1201,8 +1398,10 @@
       <c r="N13" s="8"/>
       <c r="O13" s="11"/>
       <c r="P13" s="14"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q13" s="23"/>
+      <c r="R13" s="25"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="8"/>
       <c r="C14" s="11"/>
@@ -1219,8 +1418,10 @@
       <c r="N14" s="8"/>
       <c r="O14" s="11"/>
       <c r="P14" s="14"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q14" s="23"/>
+      <c r="R14" s="25"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="8"/>
       <c r="C15" s="11"/>
@@ -1237,8 +1438,10 @@
       <c r="N15" s="8"/>
       <c r="O15" s="11"/>
       <c r="P15" s="14"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q15" s="23"/>
+      <c r="R15" s="25"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="8"/>
       <c r="C16" s="11"/>
@@ -1255,8 +1458,10 @@
       <c r="N16" s="8"/>
       <c r="O16" s="11"/>
       <c r="P16" s="14"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q16" s="23"/>
+      <c r="R16" s="25"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="8"/>
       <c r="C17" s="11"/>
@@ -1273,8 +1478,10 @@
       <c r="N17" s="8"/>
       <c r="O17" s="11"/>
       <c r="P17" s="14"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q17" s="23"/>
+      <c r="R17" s="25"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="8"/>
       <c r="C18" s="11"/>
@@ -1291,8 +1498,10 @@
       <c r="N18" s="8"/>
       <c r="O18" s="11"/>
       <c r="P18" s="14"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q18" s="23"/>
+      <c r="R18" s="25"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="8"/>
       <c r="C19" s="11"/>
@@ -1309,8 +1518,10 @@
       <c r="N19" s="8"/>
       <c r="O19" s="11"/>
       <c r="P19" s="14"/>
-    </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q19" s="23"/>
+      <c r="R19" s="25"/>
+    </row>
+    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="6"/>
       <c r="B20" s="9"/>
       <c r="C20" s="12"/>
@@ -1327,6 +1538,8 @@
       <c r="N20" s="9"/>
       <c r="O20" s="12"/>
       <c r="P20" s="15"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>